<commit_message>
fixed import, restructure, dorabotka++, warning window about import template (remains problems with export)
</commit_message>
<xml_diff>
--- a/assets/testing-files/add_orders_xls_test.xlsx
+++ b/assets/testing-files/add_orders_xls_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Documents\tgbot\pathcluster\assets\testing-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file\PyCharm Community Edition 2025.1\pathclustering_project\assets\testing-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE86148-EC25-4688-A373-9FBDE0E89FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0D457-B75B-4605-BD49-07C8E9D23519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{162BA1F8-31AD-4BDB-8BA2-12385A9A1817}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{162BA1F8-31AD-4BDB-8BA2-12385A9A1817}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Номер заказа</t>
   </si>
@@ -232,6 +232,54 @@
   </si>
   <si>
     <t>Воронеж, Пограничный пр-д, 5</t>
+  </si>
+  <si>
+    <t>89157462939</t>
+  </si>
+  <si>
+    <t>89616171966</t>
+  </si>
+  <si>
+    <t>89507656669</t>
+  </si>
+  <si>
+    <t>89802436816</t>
+  </si>
+  <si>
+    <t>89204619277</t>
+  </si>
+  <si>
+    <t>89065809980</t>
+  </si>
+  <si>
+    <t>89511549281</t>
+  </si>
+  <si>
+    <t>89805485327</t>
+  </si>
+  <si>
+    <t>89009326524</t>
+  </si>
+  <si>
+    <t>89611841424</t>
+  </si>
+  <si>
+    <t>89003075527</t>
+  </si>
+  <si>
+    <t>89525559858</t>
+  </si>
+  <si>
+    <t>89155823772</t>
+  </si>
+  <si>
+    <t>89081304789</t>
+  </si>
+  <si>
+    <t>89515672194</t>
+  </si>
+  <si>
+    <t>89204422077</t>
   </si>
 </sst>
 </file>
@@ -377,41 +425,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -430,9 +482,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -470,7 +522,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -576,7 +628,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -718,7 +770,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,7 +781,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,263 +824,263 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
-        <v>79805485327</v>
+      <c r="D2" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="F2">
         <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9">
-        <v>79009326524</v>
+      <c r="D3" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="F3">
         <v>5550</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11">
-        <v>79157462939</v>
+      <c r="D4" s="19" t="s">
+        <v>54</v>
       </c>
       <c r="F4">
         <v>8474</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9">
-        <v>79616171966</v>
+      <c r="D5" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="F5">
         <v>8858</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="14">
-        <v>79611841424</v>
+      <c r="D6" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="F6">
         <v>1135</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="14">
-        <v>79003075527</v>
+      <c r="D7" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="F7">
         <v>6400</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="14">
-        <v>79525559858</v>
+      <c r="D8" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="F8">
         <v>1314</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="9">
-        <v>79507656669</v>
+      <c r="D9" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="F9">
         <v>8903</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="14">
-        <v>79802436816</v>
+      <c r="D10" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="F10">
         <v>8561</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="16">
-        <v>79155823772</v>
+      <c r="D11" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="F11">
         <v>7453</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="14">
-        <v>79081304789</v>
+      <c r="D12" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="F12">
         <v>1565</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="18">
-        <v>79204619277</v>
+      <c r="D13" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="F13">
         <v>1234</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="19">
-        <v>79065809980</v>
+      <c r="D14" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="F14">
         <v>45364</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="16">
-        <v>79515672194</v>
+      <c r="D15" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="F15">
         <v>575800</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="14">
-        <v>79204422077</v>
+      <c r="D16" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F16">
         <v>74637</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="19">
-        <v>79511549281</v>
+      <c r="D17" s="23" t="s">
+        <v>60</v>
       </c>
       <c r="F17">
         <v>1390823</v>

</xml_diff>

<commit_message>
added error message while importing
</commit_message>
<xml_diff>
--- a/assets/testing-files/add_orders_xls_test.xlsx
+++ b/assets/testing-files/add_orders_xls_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file\PyCharm Community Edition 2025.1\pathclustering_project\assets\testing-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0D457-B75B-4605-BD49-07C8E9D23519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467BD515-F11C-474A-8927-3442CA75DF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{162BA1F8-31AD-4BDB-8BA2-12385A9A1817}"/>
   </bookViews>
@@ -255,31 +255,31 @@
     <t>89511549281</t>
   </si>
   <si>
+    <t>89009326524</t>
+  </si>
+  <si>
+    <t>89611841424</t>
+  </si>
+  <si>
+    <t>89003075527</t>
+  </si>
+  <si>
+    <t>89525559858</t>
+  </si>
+  <si>
+    <t>89155823772</t>
+  </si>
+  <si>
+    <t>89081304789</t>
+  </si>
+  <si>
+    <t>89515672194</t>
+  </si>
+  <si>
+    <t>89204422077</t>
+  </si>
+  <si>
     <t>89805485327</t>
-  </si>
-  <si>
-    <t>89009326524</t>
-  </si>
-  <si>
-    <t>89611841424</t>
-  </si>
-  <si>
-    <t>89003075527</t>
-  </si>
-  <si>
-    <t>89525559858</t>
-  </si>
-  <si>
-    <t>89155823772</t>
-  </si>
-  <si>
-    <t>89081304789</t>
-  </si>
-  <si>
-    <t>89515672194</t>
-  </si>
-  <si>
-    <t>89204422077</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241F6AEE-0460-485E-977C-0483104FF657}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F2">
         <v>1500</v>
@@ -842,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>5550</v>
@@ -893,7 +893,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6">
         <v>1135</v>
@@ -910,7 +910,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7">
         <v>6400</v>
@@ -927,7 +927,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8">
         <v>1314</v>
@@ -978,7 +978,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11">
         <v>7453</v>
@@ -995,7 +995,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12">
         <v>1565</v>
@@ -1046,7 +1046,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15">
         <v>575800</v>
@@ -1063,7 +1063,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16">
         <v>74637</v>

</xml_diff>